<commit_message>
updated the read template function.
</commit_message>
<xml_diff>
--- a/test/TEMPLATE.xlsx
+++ b/test/TEMPLATE.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>#</t>
   </si>
@@ -20,28 +20,31 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Content</t>
+  </si>
+  <si>
     <t>Location X</t>
   </si>
   <si>
     <t>Location Y</t>
   </si>
   <si>
-    <t>Text</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
     <t>Date</t>
   </si>
   <si>
+    <t>&lt;!T&gt;&lt;2024-10-25&gt;</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
     <t>Year of Assessment</t>
   </si>
   <si>
-    <t>2023/2024</t>
+    <t>&lt;!T&gt;&lt;2023/2024&gt;</t>
   </si>
   <si>
     <t>3</t>
@@ -50,13 +53,16 @@
     <t>Employers' TIN</t>
   </si>
   <si>
+    <t>&lt;!T&gt;&lt;5249087539&gt;</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
     <t>Employees Full Name</t>
   </si>
   <si>
-    <t>!&lt;PAY01.xlsx&gt;&lt;LOCKED=1&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;B&gt;</t>
+    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;LOCKED=1&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;B&gt;</t>
   </si>
   <si>
     <t>5</t>
@@ -65,22 +71,22 @@
     <t>NIC Number</t>
   </si>
   <si>
-    <t>!&lt;EMP01.xlsx&gt;&lt;LOCKED=1&gt;&lt;T9AF&gt;&lt;A&gt;&lt;B&gt;</t>
+    <t>&lt;!F&gt;&lt;EMP01.xlsx&gt;&lt;LOCKED=1&gt;&lt;T9AF&gt;&lt;A&gt;&lt;B&gt;</t>
   </si>
   <si>
     <t>!&lt;CONCAT&gt;&lt;4&gt;</t>
   </si>
   <si>
-    <t>!&lt;\20&gt;</t>
-  </si>
-  <si>
-    <t>!&lt;PAY01.xlsx&gt;&lt;LOCKED=1&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;C&gt;</t>
+    <t>&lt;!T&gt;&lt; &gt;</t>
+  </si>
+  <si>
+    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;LOCKED=1&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;C&gt;</t>
   </si>
   <si>
     <t>!&lt;CONCAT&gt;&lt;3&gt;</t>
   </si>
   <si>
-    <t>TIN</t>
+    <t>&lt;!T&gt;&lt;TIN&gt;</t>
   </si>
   <si>
     <t>Primary Ket</t>
@@ -90,9 +96,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -125,7 +130,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -150,6 +155,117 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="10"/>
       </left>
       <right style="thin">
@@ -169,7 +285,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -182,37 +298,67 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -237,54 +383,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1161016</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>153087</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1521223</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>1852</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Text"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4437616" y="3415082"/>
-          <a:ext cx="360208" cy="239926"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1343,7 +1441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1351,9 +1449,10 @@
   <cols>
     <col min="1" max="1" width="6.17188" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.1719" style="1" customWidth="1"/>
-    <col min="3" max="4" width="8.85156" style="1" customWidth="1"/>
-    <col min="5" max="5" width="47.5" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.0938" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.85156" style="1" customWidth="1"/>
+    <col min="6" max="6" width="47.5" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1372,6 +1471,7 @@
       <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
@@ -1380,158 +1480,232 @@
       <c r="B2" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" t="s" s="3">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5">
         <v>110</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="5">
         <v>95</v>
       </c>
-      <c r="E2" s="5">
-        <v>45590</v>
-      </c>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s" s="3">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5">
         <v>180</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="5">
         <v>680</v>
       </c>
-      <c r="E3" t="s" s="3">
-        <v>9</v>
-      </c>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5">
         <v>420</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="5">
         <v>680</v>
       </c>
-      <c r="E4" s="4">
-        <v>5249087539</v>
-      </c>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s" s="3">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="D5" s="5">
         <v>200</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="5">
         <v>590</v>
       </c>
-      <c r="E5" t="s" s="3">
-        <v>14</v>
-      </c>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="C6" s="4">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="D6" s="5">
         <v>420</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="5">
         <v>550</v>
       </c>
-      <c r="E6" t="s" s="3">
-        <v>17</v>
-      </c>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="6">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" t="s" s="3">
-        <v>18</v>
-      </c>
-      <c r="C7" s="4">
-        <v>-1</v>
-      </c>
-      <c r="D7" s="4">
-        <v>-1</v>
-      </c>
-      <c r="E7" t="s" s="3">
-        <v>19</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C7" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="6">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>18</v>
-      </c>
-      <c r="C8" s="4">
-        <v>-1</v>
-      </c>
-      <c r="D8" s="4">
-        <v>-1</v>
-      </c>
-      <c r="E8" t="s" s="3">
         <v>20</v>
       </c>
+      <c r="C8" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="6">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="C9" s="4">
-        <v>-1</v>
-      </c>
-      <c r="D9" s="4">
-        <v>-1</v>
-      </c>
-      <c r="E9" t="s" s="3">
-        <v>19</v>
-      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="6">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="C10" s="4">
-        <v>-1</v>
-      </c>
-      <c r="D10" s="4">
-        <v>-1</v>
-      </c>
-      <c r="E10" t="s" s="3">
-        <v>22</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C10" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="7"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" ht="15.4" customHeight="1">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" ht="15.4" customHeight="1">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" ht="15.4" customHeight="1">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" ht="15.4" customHeight="1">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" ht="15.4" customHeight="1">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" ht="15.4" customHeight="1">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" ht="15.4" customHeight="1">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" ht="15.4" customHeight="1">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" ht="15.4" customHeight="1">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="13"/>
+    </row>
+    <row r="21" ht="15.4" customHeight="1">
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1539,7 +1713,6 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1551,98 +1724,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="4.85156" style="9" customWidth="1"/>
-    <col min="2" max="2" width="15.1719" style="9" customWidth="1"/>
-    <col min="3" max="3" width="16.8516" style="9" customWidth="1"/>
-    <col min="4" max="5" width="8.85156" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="9" customWidth="1"/>
+    <col min="1" max="1" width="4.85156" style="19" customWidth="1"/>
+    <col min="2" max="2" width="15.1719" style="19" customWidth="1"/>
+    <col min="3" max="3" width="16.8516" style="19" customWidth="1"/>
+    <col min="4" max="5" width="8.85156" style="19" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="10">
+      <c r="A1" t="s" s="20">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="10">
-        <v>23</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" t="s" s="20">
+        <v>25</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="12">
+      <c r="A2" t="s" s="22">
         <v>5</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" t="s" s="22">
+        <v>8</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="13">
+      <c r="A4" s="23">
         <v>3</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="13">
+      <c r="A5" s="23">
         <v>4</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="13">
+      <c r="A6" s="23">
         <v>5</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="13">
+      <c r="A7" s="23">
         <v>6</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added the GUI functions
</commit_message>
<xml_diff>
--- a/test/TEMPLATE.xlsx
+++ b/test/TEMPLATE.xlsx
@@ -89,7 +89,7 @@
     <t>&lt;!T&gt;&lt;TIN&gt;</t>
   </si>
   <si>
-    <t>Primary Ket</t>
+    <t>Primary Key</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1449,7 @@
   <cols>
     <col min="1" max="1" width="6.17188" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.1719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.0938" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.1719" style="1" customWidth="1"/>
     <col min="4" max="5" width="8.85156" style="1" customWidth="1"/>
     <col min="6" max="6" width="47.5" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
implemented full duplex messages
</commit_message>
<xml_diff>
--- a/test/TEMPLATE.xlsx
+++ b/test/TEMPLATE.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>#</t>
   </si>
@@ -90,6 +90,48 @@
   </si>
   <si>
     <t>Primary Key</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Garcia</t>
   </si>
 </sst>
 </file>
@@ -285,7 +327,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -354,6 +396,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
@@ -1738,80 +1783,120 @@
       <c r="B1" t="s" s="20">
         <v>25</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="C1" t="s" s="20">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s" s="20">
+        <v>27</v>
+      </c>
       <c r="E1" s="21"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="22">
         <v>5</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
+      <c r="B2" s="23">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s" s="20">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s" s="20">
+        <v>29</v>
+      </c>
       <c r="E2" s="21"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="22">
         <v>8</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="B3" s="23">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s" s="20">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s" s="20">
+        <v>31</v>
+      </c>
       <c r="E3" s="21"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="23">
+      <c r="A4" s="24">
         <v>3</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
+      <c r="B4" s="23">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s" s="20">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s" s="20">
+        <v>33</v>
+      </c>
       <c r="E4" s="21"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="23">
+      <c r="A5" s="24">
         <v>4</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="23">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s" s="20">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s" s="20">
+        <v>35</v>
+      </c>
       <c r="E5" s="21"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="23">
+      <c r="A6" s="24">
         <v>5</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
+      <c r="B6" s="23">
+        <v>123</v>
+      </c>
+      <c r="C6" t="s" s="20">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s" s="20">
+        <v>37</v>
+      </c>
       <c r="E6" s="21"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="23">
+      <c r="A7" s="24">
         <v>6</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+      <c r="B7" s="23">
+        <v>124</v>
+      </c>
+      <c r="C7" t="s" s="20">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s" s="20">
+        <v>39</v>
+      </c>
       <c r="E7" s="21"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="24"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="24"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="24"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>

</xml_diff>

<commit_message>
Added the PDF functions. Removed style errors.
</commit_message>
<xml_diff>
--- a/test/TEMPLATE.xlsx
+++ b/test/TEMPLATE.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
   <si>
     <t>#</t>
   </si>
@@ -62,7 +62,7 @@
     <t>Employees Full Name</t>
   </si>
   <si>
-    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;LOCKED=1&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;B&gt;</t>
+    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;B&gt;</t>
   </si>
   <si>
     <t>5</t>
@@ -71,22 +71,28 @@
     <t>NIC Number</t>
   </si>
   <si>
-    <t>&lt;!F&gt;&lt;EMP01.xlsx&gt;&lt;LOCKED=1&gt;&lt;T9AF&gt;&lt;A&gt;&lt;B&gt;</t>
-  </si>
-  <si>
-    <t>!&lt;CONCAT&gt;&lt;4&gt;</t>
+    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;D&gt;</t>
+  </si>
+  <si>
+    <t>!&lt;CONCAT&gt;&lt;Employees Full Name&gt;</t>
   </si>
   <si>
     <t>&lt;!T&gt;&lt; &gt;</t>
   </si>
   <si>
-    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;LOCKED=1&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;C&gt;</t>
-  </si>
-  <si>
-    <t>!&lt;CONCAT&gt;&lt;3&gt;</t>
+    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;C&gt;</t>
+  </si>
+  <si>
+    <t>!&lt;CONCAT&gt;&lt;Employers' TIN&gt;</t>
   </si>
   <si>
     <t>&lt;!T&gt;&lt;TIN&gt;</t>
+  </si>
+  <si>
+    <t>Birth Day</t>
+  </si>
+  <si>
+    <t>&lt;!F&gt;&lt;EMP01.xlsx&gt;&lt;PERSONAL DATA&gt;&lt;A&gt;&lt;C&gt;</t>
   </si>
   <si>
     <t>Primary Key</t>
@@ -327,7 +333,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -354,9 +360,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -1493,7 +1496,7 @@
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="6.17188" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1719" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.8516" style="1" customWidth="1"/>
     <col min="3" max="3" width="43.1719" style="1" customWidth="1"/>
     <col min="4" max="5" width="8.85156" style="1" customWidth="1"/>
     <col min="6" max="6" width="47.5" style="1" customWidth="1"/>
@@ -1665,92 +1668,102 @@
       <c r="F10" s="6"/>
     </row>
     <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="D11" s="5">
+        <v>100</v>
+      </c>
+      <c r="E11" s="5">
+        <v>500</v>
+      </c>
       <c r="F11" s="6"/>
     </row>
     <row r="12" ht="15.4" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="13"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" ht="15.4" customHeight="1">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="13"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" ht="15.4" customHeight="1">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="13"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" ht="15.4" customHeight="1">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="13"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" ht="15.4" customHeight="1">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="13"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" ht="15.4" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="13"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="12"/>
     </row>
     <row r="18" ht="15.4" customHeight="1">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="13"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" ht="15.4" customHeight="1">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="13"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" ht="15.4" customHeight="1">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="13"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="12"/>
     </row>
     <row r="21" ht="15.4" customHeight="1">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1769,138 +1782,138 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="4.85156" style="19" customWidth="1"/>
-    <col min="2" max="2" width="15.1719" style="19" customWidth="1"/>
-    <col min="3" max="3" width="16.8516" style="19" customWidth="1"/>
-    <col min="4" max="5" width="8.85156" style="19" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="19" customWidth="1"/>
+    <col min="1" max="1" width="4.85156" style="18" customWidth="1"/>
+    <col min="2" max="2" width="15.1719" style="18" customWidth="1"/>
+    <col min="3" max="3" width="16.8516" style="18" customWidth="1"/>
+    <col min="4" max="5" width="8.85156" style="18" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="20">
+      <c r="A1" t="s" s="19">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="20">
+      <c r="B1" t="s" s="19">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s" s="19">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s" s="19">
+        <v>29</v>
+      </c>
+      <c r="E1" s="20"/>
+    </row>
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" t="s" s="21">
+        <v>5</v>
+      </c>
+      <c r="B2" s="22">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s" s="19">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s" s="19">
+        <v>31</v>
+      </c>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" t="s" s="21">
+        <v>8</v>
+      </c>
+      <c r="B3" s="22">
         <v>25</v>
       </c>
-      <c r="C1" t="s" s="20">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s" s="20">
-        <v>27</v>
-      </c>
-      <c r="E1" s="21"/>
-    </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="22">
+      <c r="C3" t="s" s="19">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="19">
+        <v>33</v>
+      </c>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="23">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s" s="19">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s" s="19">
+        <v>35</v>
+      </c>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="23">
+        <v>4</v>
+      </c>
+      <c r="B5" s="22">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s" s="19">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s" s="19">
+        <v>37</v>
+      </c>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="23">
         <v>5</v>
       </c>
-      <c r="B2" s="23">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s" s="20">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s" s="20">
-        <v>29</v>
-      </c>
-      <c r="E2" s="21"/>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="22">
-        <v>8</v>
-      </c>
-      <c r="B3" s="23">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s" s="20">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s" s="20">
-        <v>31</v>
-      </c>
-      <c r="E3" s="21"/>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="24">
-        <v>3</v>
-      </c>
-      <c r="B4" s="23">
-        <v>109</v>
-      </c>
-      <c r="C4" t="s" s="20">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s" s="20">
-        <v>33</v>
-      </c>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="24">
-        <v>4</v>
-      </c>
-      <c r="B5" s="23">
-        <v>120</v>
-      </c>
-      <c r="C5" t="s" s="20">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s" s="20">
-        <v>35</v>
-      </c>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="24">
-        <v>5</v>
-      </c>
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>123</v>
       </c>
-      <c r="C6" t="s" s="20">
-        <v>36</v>
-      </c>
-      <c r="D6" t="s" s="20">
-        <v>37</v>
-      </c>
-      <c r="E6" s="21"/>
+      <c r="C6" t="s" s="19">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s" s="19">
+        <v>39</v>
+      </c>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="24">
+      <c r="A7" s="23">
         <v>6</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="22">
         <v>124</v>
       </c>
-      <c r="C7" t="s" s="20">
-        <v>38</v>
-      </c>
-      <c r="D7" t="s" s="20">
-        <v>39</v>
-      </c>
-      <c r="E7" s="21"/>
+      <c r="C7" t="s" s="19">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s" s="19">
+        <v>41</v>
+      </c>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="25"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="25"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="25"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added PDF create function body. Removed the status UI, There is a bug in TKinter, that I can not find.
</commit_message>
<xml_diff>
--- a/test/TEMPLATE.xlsx
+++ b/test/TEMPLATE.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>#</t>
   </si>
@@ -29,85 +29,82 @@
     <t>Location Y</t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>&lt;!T&gt;&lt;2024-10-25&gt;</t>
+  </si>
+  <si>
+    <t>Year of Assessment</t>
+  </si>
+  <si>
+    <t>&lt;!T&gt;&lt;2023/2024&gt;</t>
+  </si>
+  <si>
+    <t>Employers' TIN</t>
+  </si>
+  <si>
+    <t>&lt;!T&gt;&lt;5249087539&gt;</t>
+  </si>
+  <si>
+    <t>Employees Full Name</t>
+  </si>
+  <si>
+    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;B&gt;</t>
+  </si>
+  <si>
+    <t>NIC Number</t>
+  </si>
+  <si>
+    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;D&gt;</t>
+  </si>
+  <si>
+    <t>!&lt;CONCAT&gt;&lt;Employees Full Name&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!T&gt;&lt; &gt;</t>
+  </si>
+  <si>
+    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;C&gt;</t>
+  </si>
+  <si>
+    <t>!&lt;CONCAT&gt;&lt;Employers' TIN&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!T&gt;&lt;TIN&gt;</t>
+  </si>
+  <si>
+    <t>Birth Day</t>
+  </si>
+  <si>
+    <t>&lt;!F&gt;&lt;EMP01.xlsx&gt;&lt;PERSONAL DATA&gt;&lt;A&gt;&lt;C&gt;</t>
+  </si>
+  <si>
+    <t>Date of Join</t>
+  </si>
+  <si>
+    <t>&lt;!F&gt;&lt;EMP01.xlsx&gt;&lt;PERSONAL DATA&gt;&lt;A&gt;&lt;B&gt;</t>
+  </si>
+  <si>
+    <t>Primary Key</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>&lt;!T&gt;&lt;2024-10-25&gt;</t>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
   </si>
   <si>
     <t>2</t>
-  </si>
-  <si>
-    <t>Year of Assessment</t>
-  </si>
-  <si>
-    <t>&lt;!T&gt;&lt;2023/2024&gt;</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Employers' TIN</t>
-  </si>
-  <si>
-    <t>&lt;!T&gt;&lt;5249087539&gt;</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Employees Full Name</t>
-  </si>
-  <si>
-    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;B&gt;</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>NIC Number</t>
-  </si>
-  <si>
-    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;D&gt;</t>
-  </si>
-  <si>
-    <t>!&lt;CONCAT&gt;&lt;Employees Full Name&gt;</t>
-  </si>
-  <si>
-    <t>&lt;!T&gt;&lt; &gt;</t>
-  </si>
-  <si>
-    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;C&gt;</t>
-  </si>
-  <si>
-    <t>!&lt;CONCAT&gt;&lt;Employers' TIN&gt;</t>
-  </si>
-  <si>
-    <t>&lt;!T&gt;&lt;TIN&gt;</t>
-  </si>
-  <si>
-    <t>Birth Day</t>
-  </si>
-  <si>
-    <t>&lt;!F&gt;&lt;EMP01.xlsx&gt;&lt;PERSONAL DATA&gt;&lt;A&gt;&lt;C&gt;</t>
-  </si>
-  <si>
-    <t>Primary Key</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Doe</t>
   </si>
   <si>
     <t>Jane</t>
@@ -350,13 +347,13 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -1522,183 +1519,193 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="2">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="C2" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="D2" s="6">
+        <v>110</v>
+      </c>
+      <c r="E2" s="6">
+        <v>95</v>
+      </c>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="3">
         <v>7</v>
       </c>
-      <c r="D2" s="5">
-        <v>110</v>
-      </c>
-      <c r="E2" s="5">
-        <v>95</v>
-      </c>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="2">
+      <c r="C3" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="3">
+      <c r="D3" s="6">
+        <v>180</v>
+      </c>
+      <c r="E3" s="6">
+        <v>680</v>
+      </c>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="C3" t="s" s="3">
+      <c r="C4" t="s" s="3">
         <v>10</v>
       </c>
-      <c r="D3" s="5">
-        <v>180</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="D4" s="6">
+        <v>420</v>
+      </c>
+      <c r="E4" s="6">
         <v>680</v>
       </c>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="2">
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="B4" t="s" s="3">
+      <c r="C5" t="s" s="3">
         <v>12</v>
       </c>
-      <c r="C4" t="s" s="3">
+      <c r="D5" s="6">
+        <v>200</v>
+      </c>
+      <c r="E5" s="6">
+        <v>590</v>
+      </c>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s" s="3">
         <v>13</v>
       </c>
-      <c r="D4" s="5">
+      <c r="C6" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="D6" s="6">
         <v>420</v>
       </c>
-      <c r="E4" s="5">
-        <v>680</v>
-      </c>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s" s="3">
+      <c r="E6" s="6">
+        <v>550</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s" s="3">
         <v>15</v>
       </c>
-      <c r="C5" t="s" s="3">
+      <c r="C7" t="s" s="3">
         <v>16</v>
-      </c>
-      <c r="D5" s="5">
-        <v>200</v>
-      </c>
-      <c r="E5" s="5">
-        <v>590</v>
-      </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s" s="3">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s" s="3">
-        <v>19</v>
-      </c>
-      <c r="D6" s="5">
-        <v>420</v>
-      </c>
-      <c r="E6" s="5">
-        <v>550</v>
-      </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="3">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s" s="3">
-        <v>21</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="6"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="7">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s" s="3">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="6"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="7">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" t="s" s="3">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s" s="3">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="6"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="7">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="7">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" t="s" s="3">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s" s="3">
-        <v>26</v>
-      </c>
-      <c r="D11" s="5">
+        <v>21</v>
+      </c>
+      <c r="D11" s="6">
         <v>100</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="6">
         <v>500</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" ht="15.4" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="12"/>
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="D12" s="6">
+        <v>100</v>
+      </c>
+      <c r="E12" s="6">
+        <v>600</v>
+      </c>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" ht="15.4" customHeight="1">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="12"/>
     </row>
     <row r="14" ht="15.4" customHeight="1">
@@ -1794,43 +1801,43 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="19">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s" s="19">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s" s="19">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E1" s="20"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="21">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B2" s="22">
         <v>14</v>
       </c>
       <c r="C2" t="s" s="19">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s" s="19">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2" s="20"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="21">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B3" s="22">
         <v>25</v>
       </c>
       <c r="C3" t="s" s="19">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s" s="19">
         <v>32</v>
-      </c>
-      <c r="D3" t="s" s="19">
-        <v>33</v>
       </c>
       <c r="E3" s="20"/>
     </row>
@@ -1842,10 +1849,10 @@
         <v>109</v>
       </c>
       <c r="C4" t="s" s="19">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s" s="19">
         <v>34</v>
-      </c>
-      <c r="D4" t="s" s="19">
-        <v>35</v>
       </c>
       <c r="E4" s="20"/>
     </row>
@@ -1857,10 +1864,10 @@
         <v>120</v>
       </c>
       <c r="C5" t="s" s="19">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s" s="19">
         <v>36</v>
-      </c>
-      <c r="D5" t="s" s="19">
-        <v>37</v>
       </c>
       <c r="E5" s="20"/>
     </row>
@@ -1872,10 +1879,10 @@
         <v>123</v>
       </c>
       <c r="C6" t="s" s="19">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s" s="19">
         <v>38</v>
-      </c>
-      <c r="D6" t="s" s="19">
-        <v>39</v>
       </c>
       <c r="E6" s="20"/>
     </row>
@@ -1887,10 +1894,10 @@
         <v>124</v>
       </c>
       <c r="C7" t="s" s="19">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s" s="19">
         <v>40</v>
-      </c>
-      <c r="D7" t="s" s="19">
-        <v>41</v>
       </c>
       <c r="E7" s="20"/>
     </row>

</xml_diff>

<commit_message>
Updated the file name logic.
</commit_message>
<xml_diff>
--- a/test/TEMPLATE.xlsx
+++ b/test/TEMPLATE.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
   <si>
     <t>#</t>
   </si>
@@ -95,6 +95,9 @@
     <t>Last Name</t>
   </si>
   <si>
+    <t>Identifier</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -104,6 +107,9 @@
     <t>Doe</t>
   </si>
   <si>
+    <t>John Doe</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
@@ -113,28 +119,43 @@
     <t>Smith</t>
   </si>
   <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
     <t>Michael</t>
   </si>
   <si>
     <t>Johnson</t>
   </si>
   <si>
+    <t>Michael Johnson</t>
+  </si>
+  <si>
     <t>Emily</t>
   </si>
   <si>
     <t>Brown</t>
   </si>
   <si>
+    <t>Emily Brown</t>
+  </si>
+  <si>
     <t>David</t>
   </si>
   <si>
     <t>Lee</t>
   </si>
   <si>
+    <t>David Lee</t>
+  </si>
+  <si>
     <t>Olivia</t>
   </si>
   <si>
     <t>Garcia</t>
+  </si>
+  <si>
+    <t>Olivia Garcia</t>
   </si>
 </sst>
 </file>
@@ -391,9 +412,6 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
@@ -405,6 +423,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1791,8 +1812,9 @@
   <cols>
     <col min="1" max="1" width="4.85156" style="18" customWidth="1"/>
     <col min="2" max="2" width="15.1719" style="18" customWidth="1"/>
-    <col min="3" max="3" width="16.8516" style="18" customWidth="1"/>
-    <col min="4" max="5" width="8.85156" style="18" customWidth="1"/>
+    <col min="3" max="3" width="13.2422" style="18" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="18" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="18" customWidth="1"/>
     <col min="6" max="16384" width="8.85156" style="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1809,118 +1831,138 @@
       <c r="D1" t="s" s="19">
         <v>26</v>
       </c>
-      <c r="E1" s="20"/>
+      <c r="E1" t="s" s="19">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="21">
-        <v>27</v>
-      </c>
-      <c r="B2" s="22">
+      <c r="A2" t="s" s="20">
+        <v>28</v>
+      </c>
+      <c r="B2" s="21">
         <v>14</v>
       </c>
       <c r="C2" t="s" s="19">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s" s="19">
-        <v>29</v>
-      </c>
-      <c r="E2" s="20"/>
+        <v>30</v>
+      </c>
+      <c r="E2" t="s" s="19">
+        <f>CONCATENATE(C2," ",D2)</f>
+        <v>31</v>
+      </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="21">
-        <v>30</v>
-      </c>
-      <c r="B3" s="22">
+      <c r="A3" t="s" s="20">
+        <v>32</v>
+      </c>
+      <c r="B3" s="21">
         <v>25</v>
       </c>
       <c r="C3" t="s" s="19">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s" s="19">
-        <v>32</v>
-      </c>
-      <c r="E3" s="20"/>
+        <v>34</v>
+      </c>
+      <c r="E3" t="s" s="19">
+        <f>CONCATENATE(C3," ",D3)</f>
+        <v>35</v>
+      </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="23">
+      <c r="A4" s="22">
         <v>3</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="21">
         <v>109</v>
       </c>
       <c r="C4" t="s" s="19">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s" s="19">
-        <v>34</v>
-      </c>
-      <c r="E4" s="20"/>
+        <v>37</v>
+      </c>
+      <c r="E4" t="s" s="19">
+        <f>CONCATENATE(C4," ",D4)</f>
+        <v>38</v>
+      </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="23">
+      <c r="A5" s="22">
         <v>4</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="21">
         <v>120</v>
       </c>
       <c r="C5" t="s" s="19">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s" s="19">
-        <v>36</v>
-      </c>
-      <c r="E5" s="20"/>
+        <v>40</v>
+      </c>
+      <c r="E5" t="s" s="19">
+        <f>CONCATENATE(C5," ",D5)</f>
+        <v>41</v>
+      </c>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="23">
+      <c r="A6" s="22">
         <v>5</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="21">
         <v>123</v>
       </c>
       <c r="C6" t="s" s="19">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s" s="19">
-        <v>38</v>
-      </c>
-      <c r="E6" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="E6" t="s" s="19">
+        <f>CONCATENATE(C6," ",D6)</f>
+        <v>44</v>
+      </c>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="23">
+      <c r="A7" s="22">
         <v>6</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="21">
         <v>124</v>
       </c>
       <c r="C7" t="s" s="19">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s" s="19">
-        <v>40</v>
-      </c>
-      <c r="E7" s="20"/>
+        <v>46</v>
+      </c>
+      <c r="E7" t="s" s="19">
+        <f>CONCATENATE(C7," ",D7)</f>
+        <v>47</v>
+      </c>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="24"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="24"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="24"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Implemented the font and font size changes
</commit_message>
<xml_diff>
--- a/test/TEMPLATE.xlsx
+++ b/test/TEMPLATE.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
   <si>
     <t>#</t>
   </si>
@@ -29,18 +29,27 @@
     <t>Location Y</t>
   </si>
   <si>
+    <t>Params</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
     <t>&lt;!T&gt;&lt;2024-10-25&gt;</t>
   </si>
   <si>
+    <t>&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;&lt;LineSpace=0.2X&gt;&lt;Func=Truncate&gt;&lt;Param=300,2&gt;</t>
+  </si>
+  <si>
     <t>Year of Assessment</t>
   </si>
   <si>
     <t>&lt;!T&gt;&lt;2023/2024&gt;</t>
   </si>
   <si>
+    <t>&lt;Font=Courier&gt;&lt;FontSize=10&gt;</t>
+  </si>
+  <si>
     <t>Employers' TIN</t>
   </si>
   <si>
@@ -51,6 +60,9 @@
   </si>
   <si>
     <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;B&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Font=Helvetica&gt;&lt;FontSize=16&gt;</t>
   </si>
   <si>
     <t>NIC Number</t>
@@ -196,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -217,30 +229,6 @@
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -275,15 +263,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="10"/>
       </left>
@@ -295,6 +274,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -351,7 +339,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -364,21 +352,21 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -400,31 +388,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1517,7 +1499,7 @@
     <col min="2" max="2" width="29.8516" style="1" customWidth="1"/>
     <col min="3" max="3" width="43.1719" style="1" customWidth="1"/>
     <col min="4" max="5" width="8.85156" style="1" customWidth="1"/>
-    <col min="6" max="6" width="47.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="62.8516" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1537,261 +1519,269 @@
       <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" t="s" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s" s="3">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5">
+        <v>160</v>
+      </c>
+      <c r="E2" s="5">
+        <v>442</v>
+      </c>
+      <c r="F2" t="s" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5">
+        <v>130</v>
+      </c>
+      <c r="E3" s="5">
+        <v>412</v>
+      </c>
+      <c r="F3" t="s" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5">
+        <v>170</v>
+      </c>
+      <c r="E4" s="5">
+        <v>490</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5">
+        <v>225</v>
+      </c>
+      <c r="E5" s="5">
+        <v>638</v>
+      </c>
+      <c r="F5" t="s" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="B6" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5">
+        <v>340</v>
+      </c>
+      <c r="E6" s="5">
+        <v>490</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="D2" s="6">
-        <v>160</v>
-      </c>
-      <c r="E2" s="6">
-        <v>442</v>
-      </c>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s" s="3">
+      <c r="B7" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="3">
+      <c r="B8" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="D3" s="6">
-        <v>130</v>
-      </c>
-      <c r="E3" s="6">
-        <v>412</v>
-      </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s" s="3">
+      <c r="B9" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="C4" t="s" s="3">
+      <c r="B10" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" ht="13.55" customHeight="1">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="D4" s="6">
+      <c r="B11" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="D11" s="5">
+        <v>340</v>
+      </c>
+      <c r="E11" s="5">
+        <v>515</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" ht="15.4" customHeight="1">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="D12" s="5">
         <v>170</v>
       </c>
-      <c r="E4" s="6">
-        <v>490</v>
-      </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="D5" s="6">
-        <v>225</v>
-      </c>
-      <c r="E5" s="6">
-        <v>638</v>
-      </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s" s="3">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D6" s="6">
-        <v>340</v>
-      </c>
-      <c r="E6" s="6">
-        <v>490</v>
-      </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s" s="3">
-        <v>17</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s" s="3">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s" s="3">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s" s="3">
-        <v>19</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s" s="3">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="D11" s="6">
-        <v>340</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="E12" s="5">
         <v>515</v>
       </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" ht="15.4" customHeight="1">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s" s="3">
-        <v>23</v>
-      </c>
-      <c r="D12" s="6">
-        <v>170</v>
-      </c>
-      <c r="E12" s="6">
-        <v>515</v>
-      </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" ht="15.4" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="12"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" ht="15.4" customHeight="1">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
       <c r="F14" s="12"/>
     </row>
     <row r="15" ht="15.4" customHeight="1">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
       <c r="F15" s="12"/>
     </row>
     <row r="16" ht="15.4" customHeight="1">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="11"/>
       <c r="F16" s="12"/>
     </row>
     <row r="17" ht="15.4" customHeight="1">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
       <c r="F17" s="12"/>
     </row>
     <row r="18" ht="15.4" customHeight="1">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="14"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
       <c r="F18" s="12"/>
     </row>
     <row r="19" ht="15.4" customHeight="1">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="14"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
       <c r="F19" s="12"/>
     </row>
     <row r="20" ht="15.4" customHeight="1">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
       <c r="F20" s="12"/>
     </row>
     <row r="21" ht="15.4" customHeight="1">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="17"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1810,159 +1800,159 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="4.85156" style="18" customWidth="1"/>
-    <col min="2" max="2" width="15.1719" style="18" customWidth="1"/>
-    <col min="3" max="3" width="13.2422" style="18" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="18" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="18" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="18" customWidth="1"/>
+    <col min="1" max="1" width="4.85156" style="16" customWidth="1"/>
+    <col min="2" max="2" width="15.1719" style="16" customWidth="1"/>
+    <col min="3" max="3" width="13.3516" style="16" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="16" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="19">
+      <c r="A1" t="s" s="17">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s" s="19">
+      <c r="B1" t="s" s="17">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s" s="17">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s" s="17">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s" s="17">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" t="s" s="18">
+        <v>32</v>
+      </c>
+      <c r="B2" s="19">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s" s="17">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s" s="17">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s" s="17">
+        <f>CONCATENATE(C2," ",D2)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" t="s" s="18">
+        <v>36</v>
+      </c>
+      <c r="B3" s="19">
         <v>25</v>
       </c>
-      <c r="D1" t="s" s="19">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s" s="19">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="20">
-        <v>28</v>
-      </c>
-      <c r="B2" s="21">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s" s="19">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s" s="19">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s" s="19">
-        <f>CONCATENATE(C2," ",D2)</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="20">
-        <v>32</v>
-      </c>
-      <c r="B3" s="21">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s" s="19">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s" s="19">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s" s="19">
+      <c r="C3" t="s" s="17">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s" s="17">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s" s="17">
         <f>CONCATENATE(C3," ",D3)</f>
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="22">
+      <c r="A4" s="20">
         <v>3</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="19">
         <v>109</v>
       </c>
-      <c r="C4" t="s" s="19">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s" s="19">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s" s="19">
+      <c r="C4" t="s" s="17">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s" s="17">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s" s="17">
         <f>CONCATENATE(C4," ",D4)</f>
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="22">
+      <c r="A5" s="20">
         <v>4</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="19">
         <v>120</v>
       </c>
-      <c r="C5" t="s" s="19">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s" s="19">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s" s="19">
+      <c r="C5" t="s" s="17">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s" s="17">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s" s="17">
         <f>CONCATENATE(C5," ",D5)</f>
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="22">
+      <c r="A6" s="20">
         <v>5</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="19">
         <v>123</v>
       </c>
-      <c r="C6" t="s" s="19">
-        <v>42</v>
-      </c>
-      <c r="D6" t="s" s="19">
-        <v>43</v>
-      </c>
-      <c r="E6" t="s" s="19">
+      <c r="C6" t="s" s="17">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s" s="17">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s" s="17">
         <f>CONCATENATE(C6," ",D6)</f>
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="22">
+      <c r="A7" s="20">
         <v>6</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="19">
         <v>124</v>
       </c>
-      <c r="C7" t="s" s="19">
-        <v>45</v>
-      </c>
-      <c r="D7" t="s" s="19">
-        <v>46</v>
-      </c>
-      <c r="E7" t="s" s="19">
+      <c r="C7" t="s" s="17">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s" s="17">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s" s="17">
         <f>CONCATENATE(C7," ",D7)</f>
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="23"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="23"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added Font, font size and line space parameters to line level.
</commit_message>
<xml_diff>
--- a/test/TEMPLATE.xlsx
+++ b/test/TEMPLATE.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
   <si>
     <t>#</t>
   </si>
@@ -23,22 +23,19 @@
     <t>Content</t>
   </si>
   <si>
-    <t>Location X</t>
-  </si>
-  <si>
-    <t>Location Y</t>
-  </si>
-  <si>
     <t>Params</t>
   </si>
   <si>
+    <t>PreProcess</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
     <t>&lt;!T&gt;&lt;2024-10-25&gt;</t>
   </si>
   <si>
-    <t>&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;&lt;LineSpace=0.2X&gt;&lt;Func=Truncate&gt;&lt;Param=300,2&gt;</t>
+    <t>&lt;X=160&gt;&lt;Y=442&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;</t>
   </si>
   <si>
     <t>Year of Assessment</t>
@@ -47,7 +44,7 @@
     <t>&lt;!T&gt;&lt;2023/2024&gt;</t>
   </si>
   <si>
-    <t>&lt;Font=Courier&gt;&lt;FontSize=10&gt;</t>
+    <t>&lt;X=130&gt;&lt;Y=412&gt;&lt;Font=Courier&gt;&lt;FontSize=10&gt;</t>
   </si>
   <si>
     <t>Employers' TIN</t>
@@ -56,13 +53,16 @@
     <t>&lt;!T&gt;&lt;5249087539&gt;</t>
   </si>
   <si>
+    <t>&lt;X=170&gt;&lt;Y=490&gt;&lt;Font=Courier&gt;</t>
+  </si>
+  <si>
     <t>Employees Full Name</t>
   </si>
   <si>
     <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;B&gt;</t>
   </si>
   <si>
-    <t>&lt;Font=Helvetica&gt;&lt;FontSize=16&gt;</t>
+    <t>&lt;X=225&gt;&lt;Y=638&gt;&lt;Font=Helvetica&gt;&lt;FontSize=16&gt;</t>
   </si>
   <si>
     <t>NIC Number</t>
@@ -71,6 +71,9 @@
     <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;D&gt;</t>
   </si>
   <si>
+    <t>&lt;X=340&gt;&lt;Y=490&gt;</t>
+  </si>
+  <si>
     <t>!&lt;CONCAT&gt;&lt;Employees Full Name&gt;</t>
   </si>
   <si>
@@ -92,10 +95,34 @@
     <t>&lt;!F&gt;&lt;EMP01.xlsx&gt;&lt;PERSONAL DATA&gt;&lt;A&gt;&lt;C&gt;</t>
   </si>
   <si>
+    <t>&lt;X=340&gt;&lt;Y=515&gt;</t>
+  </si>
+  <si>
     <t>Date of Join</t>
   </si>
   <si>
     <t>&lt;!F&gt;&lt;EMP01.xlsx&gt;&lt;PERSONAL DATA&gt;&lt;A&gt;&lt;B&gt;</t>
+  </si>
+  <si>
+    <t>&lt;X=170&gt;&lt;Y=515&gt;</t>
+  </si>
+  <si>
+    <t>Basic Salary</t>
+  </si>
+  <si>
+    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;E&gt;</t>
+  </si>
+  <si>
+    <t>&lt;X=170&gt;&lt;Y=200&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;&lt;Process=SrinkToFit(300,2)&gt;</t>
+  </si>
+  <si>
+    <t>&lt;PreProcess=NumberToText(text)&gt;</t>
+  </si>
+  <si>
+    <t>&lt;X=170&gt;&lt;Y=100&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;</t>
+  </si>
+  <si>
+    <t>&lt;PreProcess=NumberToCurrency(text,USD,2)&gt;</t>
   </si>
   <si>
     <t>Primary Key</t>
@@ -339,7 +366,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -354,9 +381,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -1489,18 +1513,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="6.17188" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.8516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.1719" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85156" style="1" customWidth="1"/>
-    <col min="6" max="6" width="62.8516" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.3516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.1719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="72" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.1719" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1519,67 +1543,51 @@
       <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="3">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" t="s" s="3">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="D2" t="s" s="3">
         <v>7</v>
       </c>
-      <c r="D2" s="5">
-        <v>160</v>
-      </c>
-      <c r="E2" s="5">
-        <v>442</v>
-      </c>
-      <c r="F2" t="s" s="3">
-        <v>8</v>
-      </c>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="C3" t="s" s="3">
+      <c r="D3" t="s" s="3">
         <v>10</v>
       </c>
-      <c r="D3" s="5">
-        <v>130</v>
-      </c>
-      <c r="E3" s="5">
-        <v>412</v>
-      </c>
-      <c r="F3" t="s" s="3">
-        <v>11</v>
-      </c>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s" s="3">
         <v>12</v>
       </c>
-      <c r="C4" t="s" s="3">
+      <c r="D4" t="s" s="3">
         <v>13</v>
       </c>
-      <c r="D4" s="5">
-        <v>170</v>
-      </c>
-      <c r="E4" s="5">
-        <v>490</v>
-      </c>
-      <c r="F4" s="6"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" s="4">
@@ -1591,15 +1599,10 @@
       <c r="C5" t="s" s="3">
         <v>15</v>
       </c>
-      <c r="D5" s="5">
-        <v>225</v>
-      </c>
-      <c r="E5" s="5">
-        <v>638</v>
-      </c>
-      <c r="F5" t="s" s="3">
+      <c r="D5" t="s" s="3">
         <v>16</v>
       </c>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" s="4">
@@ -1611,177 +1614,175 @@
       <c r="C6" t="s" s="3">
         <v>18</v>
       </c>
-      <c r="D6" s="5">
-        <v>340</v>
-      </c>
-      <c r="E6" s="5">
-        <v>490</v>
-      </c>
-      <c r="F6" s="6"/>
+      <c r="D6" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" t="s" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s" s="3">
-        <v>20</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s" s="3">
-        <v>20</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>23</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" ht="13.55" customHeight="1">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" t="s" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s" s="3">
-        <v>25</v>
-      </c>
-      <c r="D11" s="5">
-        <v>340</v>
-      </c>
-      <c r="E11" s="5">
-        <v>515</v>
-      </c>
-      <c r="F11" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="D11" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" ht="15.4" customHeight="1">
       <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s" s="3">
-        <v>27</v>
-      </c>
-      <c r="D12" s="5">
-        <v>170</v>
-      </c>
-      <c r="E12" s="5">
-        <v>515</v>
-      </c>
-      <c r="F12" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="D12" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" ht="15.4" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s" s="3">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s" s="3">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" ht="15.4" customHeight="1">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s" s="3">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s" s="3">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s" s="3">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" ht="15.4" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" ht="15.4" customHeight="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="9"/>
       <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
     </row>
     <row r="17" ht="15.4" customHeight="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="10"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="9"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
     </row>
     <row r="18" ht="15.4" customHeight="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="10"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="9"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
     </row>
     <row r="19" ht="15.4" customHeight="1">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="10"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
     </row>
     <row r="20" ht="15.4" customHeight="1">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="10"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
     </row>
     <row r="21" ht="15.4" customHeight="1">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="13"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1800,159 +1801,159 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="4.85156" style="16" customWidth="1"/>
-    <col min="2" max="2" width="15.1719" style="16" customWidth="1"/>
-    <col min="3" max="3" width="13.3516" style="16" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="16" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="16" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="16" customWidth="1"/>
+    <col min="1" max="1" width="4.85156" style="15" customWidth="1"/>
+    <col min="2" max="2" width="15.1719" style="15" customWidth="1"/>
+    <col min="3" max="3" width="13.3516" style="15" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="15" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="15" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="17">
+      <c r="A1" t="s" s="16">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="17">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s" s="17">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s" s="17">
-        <v>30</v>
-      </c>
-      <c r="E1" t="s" s="17">
-        <v>31</v>
+      <c r="B1" t="s" s="16">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s" s="16">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s" s="16">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s" s="16">
+        <v>40</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="18">
-        <v>32</v>
-      </c>
-      <c r="B2" s="19">
+      <c r="A2" t="s" s="17">
+        <v>41</v>
+      </c>
+      <c r="B2" s="18">
         <v>14</v>
       </c>
-      <c r="C2" t="s" s="17">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s" s="17">
-        <v>34</v>
-      </c>
-      <c r="E2" t="s" s="17">
+      <c r="C2" t="s" s="16">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s" s="16">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s" s="16">
         <f>CONCATENATE(C2," ",D2)</f>
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="18">
-        <v>36</v>
-      </c>
-      <c r="B3" s="19">
+      <c r="A3" t="s" s="17">
+        <v>45</v>
+      </c>
+      <c r="B3" s="18">
         <v>25</v>
       </c>
-      <c r="C3" t="s" s="17">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s" s="17">
-        <v>38</v>
-      </c>
-      <c r="E3" t="s" s="17">
+      <c r="C3" t="s" s="16">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s" s="16">
         <f>CONCATENATE(C3," ",D3)</f>
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="20">
+      <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="18">
         <v>109</v>
       </c>
-      <c r="C4" t="s" s="17">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s" s="17">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s" s="17">
+      <c r="C4" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s" s="16">
         <f>CONCATENATE(C4," ",D4)</f>
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="20">
+      <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <v>120</v>
       </c>
-      <c r="C5" t="s" s="17">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s" s="17">
-        <v>44</v>
-      </c>
-      <c r="E5" t="s" s="17">
+      <c r="C5" t="s" s="16">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s" s="16">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s" s="16">
         <f>CONCATENATE(C5," ",D5)</f>
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="20">
+      <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="18">
         <v>123</v>
       </c>
-      <c r="C6" t="s" s="17">
-        <v>46</v>
-      </c>
-      <c r="D6" t="s" s="17">
-        <v>47</v>
-      </c>
-      <c r="E6" t="s" s="17">
+      <c r="C6" t="s" s="16">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s" s="16">
+        <v>56</v>
+      </c>
+      <c r="E6" t="s" s="16">
         <f>CONCATENATE(C6," ",D6)</f>
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="20">
+      <c r="A7" s="19">
         <v>6</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="18">
         <v>124</v>
       </c>
-      <c r="C7" t="s" s="17">
-        <v>49</v>
-      </c>
-      <c r="D7" t="s" s="17">
-        <v>50</v>
-      </c>
-      <c r="E7" t="s" s="17">
+      <c r="C7" t="s" s="16">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s" s="16">
+        <v>59</v>
+      </c>
+      <c r="E7" t="s" s="16">
         <f>CONCATENATE(C7," ",D7)</f>
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="21"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
UPDATED THE NEW TEMPLATE FORMAT (MAJOR CHANGE)
</commit_message>
<xml_diff>
--- a/test/TEMPLATE.xlsx
+++ b/test/TEMPLATE.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
   <si>
     <t>#</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>&lt;!T&gt;&lt;2024-10-25&gt;</t>
+    <t>&lt;Type=Text&gt;&lt;Text=2024-10-25&gt;</t>
   </si>
   <si>
     <t>&lt;X=160&gt;&lt;Y=442&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;</t>
@@ -41,7 +41,7 @@
     <t>Year of Assessment</t>
   </si>
   <si>
-    <t>&lt;!T&gt;&lt;2023/2024&gt;</t>
+    <t>&lt;Type=Text&gt;&lt;Text=2023/2024&gt;</t>
   </si>
   <si>
     <t>&lt;X=130&gt;&lt;Y=412&gt;&lt;Font=Courier&gt;&lt;FontSize=10&gt;</t>
@@ -50,7 +50,7 @@
     <t>Employers' TIN</t>
   </si>
   <si>
-    <t>&lt;!T&gt;&lt;5249087539&gt;</t>
+    <t>&lt;Type=Text&gt;&lt;Text=5249087539&gt;</t>
   </si>
   <si>
     <t>&lt;X=170&gt;&lt;Y=490&gt;&lt;Font=Courier&gt;</t>
@@ -59,7 +59,7 @@
     <t>Employees Full Name</t>
   </si>
   <si>
-    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;B&gt;</t>
+    <t>&lt;Type=File&gt;&lt;File=PAY01.xlsx&gt;&lt;Sheet=SALERY DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=B&gt;</t>
   </si>
   <si>
     <t>&lt;X=225&gt;&lt;Y=638&gt;&lt;Font=Helvetica&gt;&lt;FontSize=16&gt;</t>
@@ -68,7 +68,7 @@
     <t>NIC Number</t>
   </si>
   <si>
-    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;D&gt;</t>
+    <t>&lt;Type=File&gt;&lt;File=PAY01.xlsx&gt;&lt;Sheet=SALERY DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=D&gt;</t>
   </si>
   <si>
     <t>&lt;X=340&gt;&lt;Y=490&gt;</t>
@@ -77,22 +77,25 @@
     <t>!&lt;CONCAT&gt;&lt;Employees Full Name&gt;</t>
   </si>
   <si>
-    <t>&lt;!T&gt;&lt; &gt;</t>
-  </si>
-  <si>
-    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;C&gt;</t>
+    <t>&lt;Type=Text&gt;&lt;Text=&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Function=AddSpace(None)&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Type=File&gt;&lt;File=PAY01.xlsx&gt;&lt;Sheet=SALERY DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=C&gt;</t>
   </si>
   <si>
     <t>!&lt;CONCAT&gt;&lt;Employers' TIN&gt;</t>
   </si>
   <si>
-    <t>&lt;!T&gt;&lt;TIN&gt;</t>
+    <t>&lt;Type=Text&gt;&lt;Text=TIN&gt;</t>
   </si>
   <si>
     <t>Birth Day</t>
   </si>
   <si>
-    <t>&lt;!F&gt;&lt;EMP01.xlsx&gt;&lt;PERSONAL DATA&gt;&lt;A&gt;&lt;C&gt;</t>
+    <t>&lt;Type=File&gt;&lt;File=EMP01.xlsx&gt;&lt;Sheet=PERSONAL DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=C&gt;</t>
   </si>
   <si>
     <t>&lt;X=340&gt;&lt;Y=515&gt;</t>
@@ -101,7 +104,7 @@
     <t>Date of Join</t>
   </si>
   <si>
-    <t>&lt;!F&gt;&lt;EMP01.xlsx&gt;&lt;PERSONAL DATA&gt;&lt;A&gt;&lt;B&gt;</t>
+    <t>&lt;Type=File&gt;&lt;File=EMP01.xlsx&gt;&lt;Sheet=PERSONAL DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=B&gt;</t>
   </si>
   <si>
     <t>&lt;X=170&gt;&lt;Y=515&gt;</t>
@@ -110,19 +113,19 @@
     <t>Basic Salary</t>
   </si>
   <si>
-    <t>&lt;!F&gt;&lt;PAY01.xlsx&gt;&lt;SALERY DATA&gt;&lt;A&gt;&lt;E&gt;</t>
-  </si>
-  <si>
-    <t>&lt;X=170&gt;&lt;Y=200&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;&lt;Process=SrinkToFit(300,2)&gt;</t>
-  </si>
-  <si>
-    <t>&lt;PreProcess=NumberToText(text)&gt;</t>
+    <t>&lt;Type=File&gt;&lt;File=PAY01.xlsx&gt;&lt;Sheet=SALERY DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=E&gt;</t>
+  </si>
+  <si>
+    <t>&lt;X=170&gt;&lt;Y=200&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;&lt;Function=SrinkToFit(300,2)&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Function=NumberToText(text)&gt;</t>
   </si>
   <si>
     <t>&lt;X=170&gt;&lt;Y=100&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;</t>
   </si>
   <si>
-    <t>&lt;PreProcess=NumberToCurrency(text,USD,2)&gt;</t>
+    <t>&lt;Function=NumberToCurrency(text,USD,2)&gt;</t>
   </si>
   <si>
     <t>Primary Key</t>
@@ -1521,7 +1524,7 @@
   <cols>
     <col min="1" max="1" width="6.17188" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.1719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="62.8516" style="1" customWidth="1"/>
     <col min="4" max="4" width="72" style="1" customWidth="1"/>
     <col min="5" max="5" width="45.1719" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
@@ -1630,7 +1633,9 @@
         <v>21</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="E7" t="s" s="3">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" s="4">
@@ -1640,7 +1645,7 @@
         <v>20</v>
       </c>
       <c r="C8" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1650,23 +1655,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s" s="3">
         <v>21</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="E9" t="s" s="3">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1676,13 +1683,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E11" s="5"/>
     </row>
@@ -1691,13 +1698,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E12" s="5"/>
     </row>
@@ -1706,16 +1713,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s" s="3">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" ht="15.4" customHeight="1">
@@ -1723,16 +1730,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" ht="15.4" customHeight="1">
@@ -1814,52 +1821,52 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="16">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s" s="16">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s" s="16">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s" s="16">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="17">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" s="18">
         <v>14</v>
       </c>
       <c r="C2" t="s" s="16">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s" s="16">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s" s="16">
         <f>CONCATENATE(C2," ",D2)</f>
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="17">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B3" s="18">
         <v>25</v>
       </c>
       <c r="C3" t="s" s="16">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s" s="16">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s" s="16">
         <f>CONCATENATE(C3," ",D3)</f>
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
@@ -1870,14 +1877,14 @@
         <v>109</v>
       </c>
       <c r="C4" t="s" s="16">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s" s="16">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s" s="16">
         <f>CONCATENATE(C4," ",D4)</f>
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
@@ -1888,14 +1895,14 @@
         <v>120</v>
       </c>
       <c r="C5" t="s" s="16">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s" s="16">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s" s="16">
         <f>CONCATENATE(C5," ",D5)</f>
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" ht="13.55" customHeight="1">
@@ -1906,14 +1913,14 @@
         <v>123</v>
       </c>
       <c r="C6" t="s" s="16">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s" s="16">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s" s="16">
         <f>CONCATENATE(C6," ",D6)</f>
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" ht="13.55" customHeight="1">
@@ -1924,14 +1931,14 @@
         <v>124</v>
       </c>
       <c r="C7" t="s" s="16">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s" s="16">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s" s="16">
         <f>CONCATENATE(C7," ",D7)</f>
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" ht="13.55" customHeight="1">

</xml_diff>

<commit_message>
Release candidate V 1.0
</commit_message>
<xml_diff>
--- a/test/TEMPLATE.xlsx
+++ b/test/TEMPLATE.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
   <si>
     <t>#</t>
   </si>
@@ -35,7 +35,7 @@
     <t>&lt;Type=Text&gt;&lt;Text=2024-10-25&gt;</t>
   </si>
   <si>
-    <t>&lt;X=160&gt;&lt;Y=442&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;</t>
+    <t>&lt;X=160&gt;&lt;Y=442&gt;</t>
   </si>
   <si>
     <t>Year of Assessment</t>
@@ -65,13 +65,19 @@
     <t>&lt;X=225&gt;&lt;Y=638&gt;&lt;Font=Helvetica&gt;&lt;FontSize=16&gt;</t>
   </si>
   <si>
+    <t>&lt;Function=AddSpace(text,1)&gt;</t>
+  </si>
+  <si>
     <t>NIC Number</t>
   </si>
   <si>
     <t>&lt;Type=File&gt;&lt;File=PAY01.xlsx&gt;&lt;Sheet=SALERY DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=D&gt;</t>
   </si>
   <si>
-    <t>&lt;X=340&gt;&lt;Y=490&gt;</t>
+    <t>&lt;X=340&gt;&lt;Y=490&gt;&lt;Font=Courier&gt;</t>
+  </si>
+  <si>
+    <t>SKIP</t>
   </si>
   <si>
     <t>!&lt;CONCAT&gt;&lt;Employees Full Name&gt;</t>
@@ -80,9 +86,6 @@
     <t>&lt;Type=Text&gt;&lt;Text=&gt;</t>
   </si>
   <si>
-    <t>&lt;Function=AddSpace(None)&gt;</t>
-  </si>
-  <si>
     <t>&lt;Type=File&gt;&lt;File=PAY01.xlsx&gt;&lt;Sheet=SALERY DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=C&gt;</t>
   </si>
   <si>
@@ -110,22 +113,61 @@
     <t>&lt;X=170&gt;&lt;Y=515&gt;</t>
   </si>
   <si>
+    <t>Basic Salary in Words</t>
+  </si>
+  <si>
+    <t>&lt;Type=File&gt;&lt;File=PAY01.xlsx&gt;&lt;Sheet=SALERY DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=E&gt;</t>
+  </si>
+  <si>
+    <t>&lt;X=1.01in&gt;&lt;Y=8.2in&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;&lt;Function=SrinkToFit(4.2in,2)&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Function=NumberToText(text,Integer)&gt;</t>
+  </si>
+  <si>
     <t>Basic Salary</t>
   </si>
   <si>
-    <t>&lt;Type=File&gt;&lt;File=PAY01.xlsx&gt;&lt;Sheet=SALERY DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=E&gt;</t>
-  </si>
-  <si>
-    <t>&lt;X=170&gt;&lt;Y=200&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;&lt;Function=SrinkToFit(300,2)&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Function=NumberToText(text)&gt;</t>
-  </si>
-  <si>
-    <t>&lt;X=170&gt;&lt;Y=100&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;</t>
+    <t>&lt;X=25mm&gt;&lt;Y=215mm&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;</t>
   </si>
   <si>
     <t>&lt;Function=NumberToCurrency(text,USD,2)&gt;</t>
+  </si>
+  <si>
+    <t>Calibration 0 0</t>
+  </si>
+  <si>
+    <t>&lt;Type=Text&gt;&lt;Text=L [Zero]&gt;</t>
+  </si>
+  <si>
+    <t>&lt;X=0&gt;&lt;Y=0&gt;&lt;Font=Courier&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;</t>
+  </si>
+  <si>
+    <t>Calibration 505 504</t>
+  </si>
+  <si>
+    <t>&lt;Type=Text&gt;&lt;Text=L [504]&gt;</t>
+  </si>
+  <si>
+    <t>&lt;X=500&gt;&lt;Y=500&gt;&lt;Font=Courier&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;</t>
+  </si>
+  <si>
+    <t>Calibration 4 inch</t>
+  </si>
+  <si>
+    <t>&lt;Type=Text&gt;&lt;Text=L 4 INCH&gt;</t>
+  </si>
+  <si>
+    <t>&lt;X=4in&gt;&lt;Y=4in&gt;&lt;Font=Courier&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;</t>
+  </si>
+  <si>
+    <t>Calibration 30 mm</t>
+  </si>
+  <si>
+    <t>&lt;Type=Text&gt;&lt;Text=L 30MM&gt;</t>
+  </si>
+  <si>
+    <t>&lt;X=30mm&gt;&lt;Y=30mm&gt;&lt;Font=Courier&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;</t>
   </si>
   <si>
     <t>Primary Key</t>
@@ -1525,7 +1567,7 @@
     <col min="1" max="1" width="6.17188" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.3516" style="1" customWidth="1"/>
     <col min="3" max="3" width="62.8516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="72" style="1" customWidth="1"/>
+    <col min="4" max="4" width="90.2266" style="1" customWidth="1"/>
     <col min="5" max="5" width="45.1719" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
@@ -1605,36 +1647,38 @@
       <c r="D5" t="s" s="3">
         <v>16</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" t="s" s="3">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="4">
-        <v>6</v>
+      <c r="A7" t="s" s="2">
+        <v>21</v>
       </c>
       <c r="B7" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s" s="3">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" t="s" s="3">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" ht="13.55" customHeight="1">
@@ -1642,10 +1686,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1655,14 +1699,14 @@
         <v>8</v>
       </c>
       <c r="B9" t="s" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s" s="3">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" t="s" s="3">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" ht="13.55" customHeight="1">
@@ -1670,10 +1714,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1683,13 +1727,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E11" s="5"/>
     </row>
@@ -1698,13 +1742,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E12" s="5"/>
     </row>
@@ -1713,16 +1757,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s" s="3">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" ht="15.4" customHeight="1">
@@ -1730,52 +1774,84 @@
         <v>13</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s" s="3">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s" s="3">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" ht="15.4" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="8"/>
+      <c r="A15" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s" s="3">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s" s="3">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s" s="3">
+        <v>42</v>
+      </c>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" ht="15.4" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="11"/>
+      <c r="A16" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s" s="3">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s" s="3">
+        <v>45</v>
+      </c>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" ht="15.4" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="11"/>
+      <c r="A17" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s" s="3">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s" s="3">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s" s="3">
+        <v>48</v>
+      </c>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" ht="15.4" customHeight="1">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="11"/>
+      <c r="A18" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s" s="3">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s" s="3">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s" s="3">
+        <v>51</v>
+      </c>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" ht="15.4" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="11"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" ht="15.4" customHeight="1">
       <c r="A20" s="9"/>
@@ -1821,52 +1897,52 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="16">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s" s="16">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s" s="16">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s" s="16">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="17">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B2" s="18">
         <v>14</v>
       </c>
       <c r="C2" t="s" s="16">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s" s="16">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s" s="16">
         <f>CONCATENATE(C2," ",D2)</f>
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="17">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B3" s="18">
         <v>25</v>
       </c>
       <c r="C3" t="s" s="16">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s" s="16">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s" s="16">
         <f>CONCATENATE(C3," ",D3)</f>
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
@@ -1877,14 +1953,14 @@
         <v>109</v>
       </c>
       <c r="C4" t="s" s="16">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s" s="16">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s" s="16">
         <f>CONCATENATE(C4," ",D4)</f>
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
@@ -1895,14 +1971,14 @@
         <v>120</v>
       </c>
       <c r="C5" t="s" s="16">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s" s="16">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s" s="16">
         <f>CONCATENATE(C5," ",D5)</f>
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" ht="13.55" customHeight="1">
@@ -1913,14 +1989,14 @@
         <v>123</v>
       </c>
       <c r="C6" t="s" s="16">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s" s="16">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s" s="16">
         <f>CONCATENATE(C6," ",D6)</f>
-        <v>58</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" ht="13.55" customHeight="1">
@@ -1931,14 +2007,14 @@
         <v>124</v>
       </c>
       <c r="C7" t="s" s="16">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s" s="16">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s" s="16">
         <f>CONCATENATE(C7," ",D7)</f>
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" ht="13.55" customHeight="1">

</xml_diff>

<commit_message>
Added support for case conversion for text.
</commit_message>
<xml_diff>
--- a/test/TEMPLATE.xlsx
+++ b/test/TEMPLATE.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="85">
   <si>
     <t>#</t>
   </si>
@@ -168,6 +168,33 @@
   </si>
   <si>
     <t>&lt;X=30mm&gt;&lt;Y=30mm&gt;&lt;Font=Courier&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;</t>
+  </si>
+  <si>
+    <t>Case Test</t>
+  </si>
+  <si>
+    <t>&lt;Type=Text&gt;&lt;Text=Case Change Text Lower = &gt;</t>
+  </si>
+  <si>
+    <t>&lt;X=25&gt;&lt;Y=390&gt;</t>
+  </si>
+  <si>
+    <t>!&lt;CONCAT&gt;&lt;Case Test&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Function=changeTextCase(text,lower)&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Type=Text&gt;&lt;Text=, Upper = &gt;</t>
+  </si>
+  <si>
+    <t>&lt;Function=changeTextCase(text,UPPER)&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Type=Text&gt;&lt;Text=, Title = &gt;</t>
+  </si>
+  <si>
+    <t>&lt;Function=changeTextCase(text,Title)&gt;</t>
   </si>
   <si>
     <t>Primary Key</t>
@@ -280,7 +307,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -307,93 +334,6 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -411,7 +351,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -430,52 +370,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1558,7 +1471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1567,7 +1480,7 @@
     <col min="1" max="1" width="6.17188" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.3516" style="1" customWidth="1"/>
     <col min="3" max="3" width="62.8516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="90.2266" style="1" customWidth="1"/>
+    <col min="4" max="4" width="90.1719" style="1" customWidth="1"/>
     <col min="5" max="5" width="45.1719" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
@@ -1847,25 +1760,96 @@
       <c r="E18" s="5"/>
     </row>
     <row r="19" ht="15.4" customHeight="1">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="8"/>
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s" s="3">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s" s="3">
+        <v>53</v>
+      </c>
+      <c r="D19" t="s" s="3">
+        <v>54</v>
+      </c>
+      <c r="E19" t="s" s="3">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" ht="15.4" customHeight="1">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="11"/>
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" t="s" s="3">
+        <v>56</v>
+      </c>
     </row>
     <row r="21" ht="15.4" customHeight="1">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="14"/>
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" t="s" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" ht="15.4" customHeight="1">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" t="s" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" ht="15.4" customHeight="1">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s" s="3">
+        <v>59</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" t="s" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" ht="15.4" customHeight="1">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" t="s" s="3">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1884,159 +1868,159 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="4.85156" style="15" customWidth="1"/>
-    <col min="2" max="2" width="15.1719" style="15" customWidth="1"/>
-    <col min="3" max="3" width="13.3516" style="15" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="15" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="15" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="15" customWidth="1"/>
+    <col min="1" max="1" width="4.85156" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.1719" style="6" customWidth="1"/>
+    <col min="3" max="3" width="13.3516" style="6" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="16">
+      <c r="A1" t="s" s="7">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="16">
-        <v>52</v>
-      </c>
-      <c r="C1" t="s" s="16">
-        <v>53</v>
-      </c>
-      <c r="D1" t="s" s="16">
-        <v>54</v>
-      </c>
-      <c r="E1" t="s" s="16">
-        <v>55</v>
+      <c r="B1" t="s" s="7">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s" s="7">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s" s="7">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s" s="7">
+        <v>64</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="17">
-        <v>56</v>
-      </c>
-      <c r="B2" s="18">
+      <c r="A2" t="s" s="8">
+        <v>65</v>
+      </c>
+      <c r="B2" s="9">
         <v>14</v>
       </c>
-      <c r="C2" t="s" s="16">
-        <v>57</v>
-      </c>
-      <c r="D2" t="s" s="16">
-        <v>58</v>
-      </c>
-      <c r="E2" t="s" s="16">
+      <c r="C2" t="s" s="7">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s" s="7">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s" s="7">
         <f>CONCATENATE(C2," ",D2)</f>
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="17">
-        <v>60</v>
-      </c>
-      <c r="B3" s="18">
+      <c r="A3" t="s" s="8">
+        <v>69</v>
+      </c>
+      <c r="B3" s="9">
         <v>25</v>
       </c>
-      <c r="C3" t="s" s="16">
-        <v>61</v>
-      </c>
-      <c r="D3" t="s" s="16">
-        <v>62</v>
-      </c>
-      <c r="E3" t="s" s="16">
+      <c r="C3" t="s" s="7">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s" s="7">
         <f>CONCATENATE(C3," ",D3)</f>
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="19">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="9">
         <v>109</v>
       </c>
-      <c r="C4" t="s" s="16">
-        <v>64</v>
-      </c>
-      <c r="D4" t="s" s="16">
-        <v>65</v>
-      </c>
-      <c r="E4" t="s" s="16">
+      <c r="C4" t="s" s="7">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s" s="7">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s" s="7">
         <f>CONCATENATE(C4," ",D4)</f>
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="19">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="9">
         <v>120</v>
       </c>
-      <c r="C5" t="s" s="16">
-        <v>67</v>
-      </c>
-      <c r="D5" t="s" s="16">
-        <v>68</v>
-      </c>
-      <c r="E5" t="s" s="16">
+      <c r="C5" t="s" s="7">
+        <v>76</v>
+      </c>
+      <c r="D5" t="s" s="7">
+        <v>77</v>
+      </c>
+      <c r="E5" t="s" s="7">
         <f>CONCATENATE(C5," ",D5)</f>
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="19">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="9">
         <v>123</v>
       </c>
-      <c r="C6" t="s" s="16">
-        <v>70</v>
-      </c>
-      <c r="D6" t="s" s="16">
-        <v>71</v>
-      </c>
-      <c r="E6" t="s" s="16">
+      <c r="C6" t="s" s="7">
+        <v>79</v>
+      </c>
+      <c r="D6" t="s" s="7">
+        <v>80</v>
+      </c>
+      <c r="E6" t="s" s="7">
         <f>CONCATENATE(C6," ",D6)</f>
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="19">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="9">
         <v>124</v>
       </c>
-      <c r="C7" t="s" s="16">
-        <v>73</v>
-      </c>
-      <c r="D7" t="s" s="16">
-        <v>74</v>
-      </c>
-      <c r="E7" t="s" s="16">
+      <c r="C7" t="s" s="7">
+        <v>82</v>
+      </c>
+      <c r="D7" t="s" s="7">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s" s="7">
         <f>CONCATENATE(C7," ",D7)</f>
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated the test files to recreate the date format bug and the decimal point drop bug.
</commit_message>
<xml_diff>
--- a/test/TEMPLATE.xlsx
+++ b/test/TEMPLATE.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82e6af1bc8f9bb0d/Documents/PDF_OVERLAY/test/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_406D1396F073FC371320E0270D17ABE55B66D58B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75B6A8ED-B9D7-453D-9971-58451E33378A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Overlay" sheetId="1" r:id="rId4"/>
-    <sheet name="Data" sheetId="2" r:id="rId5"/>
+    <sheet name="Overlay" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="191029" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
   <si>
     <t>#</t>
   </si>
@@ -218,9 +227,6 @@
     <t>Doe</t>
   </si>
   <si>
-    <t>John Doe</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -230,65 +236,49 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>Jane Smith</t>
-  </si>
-  <si>
     <t>Michael</t>
   </si>
   <si>
     <t>Johnson</t>
   </si>
   <si>
-    <t>Michael Johnson</t>
-  </si>
-  <si>
     <t>Emily</t>
   </si>
   <si>
     <t>Brown</t>
   </si>
   <si>
-    <t>Emily Brown</t>
-  </si>
-  <si>
     <t>David</t>
   </si>
   <si>
     <t>Lee</t>
   </si>
   <si>
-    <t>David Lee</t>
-  </si>
-  <si>
     <t>Olivia</t>
   </si>
   <si>
     <t>Garcia</t>
   </si>
   <si>
-    <t>Olivia Garcia</t>
+    <t>Zero</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>&lt;Type=Text&gt;&lt;Text=0.00&gt;</t>
+  </si>
+  <si>
+    <t>&lt;X=360&gt;&lt;Y=442&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -347,50 +337,31 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,24 +370,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -542,7 +574,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -551,7 +583,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -560,7 +592,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -634,7 +666,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -642,7 +674,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -660,7 +692,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -689,7 +721,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -714,7 +746,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -739,7 +771,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -764,7 +796,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -789,7 +821,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -814,7 +846,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -839,7 +871,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -864,7 +896,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -889,7 +921,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -902,9 +934,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -919,7 +957,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -927,7 +965,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -945,7 +983,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -970,7 +1008,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -995,7 +1033,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1020,7 +1058,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1045,7 +1083,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1070,7 +1108,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1095,7 +1133,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1120,7 +1158,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1145,7 +1183,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1170,7 +1208,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1183,9 +1221,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1199,7 +1243,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1217,7 +1261,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1246,7 +1290,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1271,7 +1315,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1296,7 +1340,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1321,7 +1365,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1346,7 +1390,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1371,7 +1415,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1396,7 +1440,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1421,7 +1465,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1446,7 +1490,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1459,401 +1503,413 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.45" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.17188" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="62.8516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="90.1719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="45.1719" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="62.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="90.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="13.55" customHeight="1">
+    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" ht="13.55" customHeight="1">
+    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="3">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s" s="3">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s" s="3">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" ht="13.55" customHeight="1">
+    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="3">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s" s="3">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s" s="3">
+      <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" ht="13.55" customHeight="1">
+    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="3">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s" s="3">
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s" s="3">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s" s="3">
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" ht="13.55" customHeight="1">
+    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="3">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s" s="3">
+      <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s" s="3">
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s" s="3">
-        <v>23</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" t="s" s="3">
+    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" ht="13.55" customHeight="1">
+    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="3">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s" s="3">
+      <c r="C8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" ht="13.55" customHeight="1">
+    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="3">
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s" s="3">
+      <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="E9" t="s" s="3">
+      <c r="E9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" ht="13.55" customHeight="1">
+    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" t="s" s="3">
+      <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s" s="3">
+      <c r="C10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" ht="13.55" customHeight="1">
+    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" t="s" s="3">
+      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s" s="3">
+      <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s" s="3">
+      <c r="D11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" ht="15.4" customHeight="1">
+    <row r="12" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" t="s" s="3">
+      <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s" s="3">
+      <c r="C12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D12" t="s" s="3">
+      <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" ht="15.4" customHeight="1">
+    <row r="13" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" t="s" s="3">
+      <c r="B13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C13" t="s" s="3">
+      <c r="C13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s" s="3">
+      <c r="D13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E13" t="s" s="3">
+      <c r="E13" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" ht="15.4" customHeight="1">
+    <row r="14" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" t="s" s="3">
+      <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C14" t="s" s="3">
+      <c r="C14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D14" t="s" s="3">
+      <c r="D14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E14" t="s" s="3">
+      <c r="E14" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" ht="15.4" customHeight="1">
-      <c r="A15" t="s" s="2">
+    <row r="15" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s" s="3">
+      <c r="B15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C15" t="s" s="3">
+      <c r="C15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D15" t="s" s="3">
+      <c r="D15" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" ht="15.4" customHeight="1">
-      <c r="A16" t="s" s="2">
+    <row r="16" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="s" s="3">
+      <c r="B16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C16" t="s" s="3">
+      <c r="C16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D16" t="s" s="3">
+      <c r="D16" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" ht="15.4" customHeight="1">
-      <c r="A17" t="s" s="2">
+    <row r="17" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="s" s="3">
+      <c r="B17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C17" t="s" s="3">
+      <c r="C17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D17" t="s" s="3">
+      <c r="D17" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" ht="15.4" customHeight="1">
-      <c r="A18" t="s" s="2">
+    <row r="18" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s" s="3">
+      <c r="B18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C18" t="s" s="3">
+      <c r="C18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D18" t="s" s="3">
+      <c r="D18" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" ht="15.4" customHeight="1">
+    <row r="19" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" t="s" s="3">
+      <c r="B19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C19" t="s" s="3">
+      <c r="C19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D19" t="s" s="3">
+      <c r="D19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E19" t="s" s="3">
+      <c r="E19" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" ht="15.4" customHeight="1">
+    <row r="20" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" t="s" s="3">
+      <c r="B20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C20" t="s" s="3">
+      <c r="C20" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="3"/>
-      <c r="E20" t="s" s="3">
+      <c r="E20" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" ht="15.4" customHeight="1">
+    <row r="21" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" t="s" s="3">
+      <c r="B21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C21" t="s" s="3">
+      <c r="C21" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D21" s="3"/>
-      <c r="E21" t="s" s="3">
+      <c r="E21" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" ht="15.4" customHeight="1">
+    <row r="22" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" t="s" s="3">
+      <c r="B22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C22" t="s" s="3">
+      <c r="C22" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="3"/>
-      <c r="E22" t="s" s="3">
+      <c r="E22" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" ht="15.4" customHeight="1">
+    <row r="23" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" t="s" s="3">
+      <c r="B23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C23" t="s" s="3">
+      <c r="C23" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D23" s="3"/>
-      <c r="E23" t="s" s="3">
+      <c r="E23" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" ht="15.4" customHeight="1">
+    <row r="24" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" t="s" s="3">
+      <c r="B24" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C24" t="s" s="3">
+      <c r="C24" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="3"/>
-      <c r="E24" t="s" s="3">
+      <c r="E24" s="3" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1861,170 +1917,171 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.45" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85156" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15.1719" style="6" customWidth="1"/>
-    <col min="3" max="3" width="13.3516" style="6" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="6" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="7">
+    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="7">
+      <c r="B1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s" s="7">
+      <c r="C1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D1" t="s" s="7">
+      <c r="D1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s" s="7">
+      <c r="E1" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="8">
+    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>14</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="C2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D2" t="s" s="7">
+      <c r="D2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E2" t="s" s="7">
-        <f>CONCATENATE(C2," ",D2)</f>
+      <c r="E2" s="6" t="str">
+        <f t="shared" ref="E2:E7" si="0">CONCATENATE(C2," ",D2)</f>
+        <v>John Doe</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="8">
+      <c r="B3" s="8">
+        <v>25</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="9">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s" s="7">
+      <c r="D3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="E3" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Jane Smith</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>109</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E3" t="s" s="7">
-        <f>CONCATENATE(C3," ",D3)</f>
+      <c r="D4" s="6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="10">
-        <v>3</v>
-      </c>
-      <c r="B4" s="9">
-        <v>109</v>
-      </c>
-      <c r="C4" t="s" s="7">
+      <c r="E4" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Michael Johnson</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>120</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D4" t="s" s="7">
+      <c r="D5" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E4" t="s" s="7">
-        <f>CONCATENATE(C4," ",D4)</f>
+      <c r="E5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Emily Brown</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8">
+        <v>123</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" s="9">
-        <v>120</v>
-      </c>
-      <c r="C5" t="s" s="7">
+      <c r="D6" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D5" t="s" s="7">
+      <c r="E6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>David Lee</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8">
+        <v>124</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E5" t="s" s="7">
-        <f>CONCATENATE(C5," ",D5)</f>
+      <c r="D7" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="10">
-        <v>5</v>
-      </c>
-      <c r="B6" s="9">
-        <v>123</v>
-      </c>
-      <c r="C6" t="s" s="7">
-        <v>79</v>
-      </c>
-      <c r="D6" t="s" s="7">
-        <v>80</v>
-      </c>
-      <c r="E6" t="s" s="7">
-        <f>CONCATENATE(C6," ",D6)</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="10">
-        <v>6</v>
-      </c>
-      <c r="B7" s="9">
-        <v>124</v>
-      </c>
-      <c r="C7" t="s" s="7">
-        <v>82</v>
-      </c>
-      <c r="D7" t="s" s="7">
-        <v>83</v>
-      </c>
-      <c r="E7" t="s" s="7">
-        <f>CONCATENATE(C7," ",D7)</f>
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
+      <c r="E7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Olivia Garcia</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Added two "pre-proccesor" functions
</commit_message>
<xml_diff>
--- a/test/TEMPLATE.xlsx
+++ b/test/TEMPLATE.xlsx
@@ -1,27 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82e6af1bc8f9bb0d/Documents/PDF_OVERLAY/test/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_406D1396F073FC371320E0270D17ABE55B66D58B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75B6A8ED-B9D7-453D-9971-58451E33378A}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Overlay" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Overlay" sheetId="1" r:id="rId4"/>
+    <sheet name="Data" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
   <si>
     <t>#</t>
   </si>
@@ -86,63 +77,93 @@
     <t>&lt;X=340&gt;&lt;Y=490&gt;&lt;Font=Courier&gt;</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>PrintZero</t>
+  </si>
+  <si>
+    <t>&lt;Type=Text&gt;&lt;Text=0.00&gt;</t>
+  </si>
+  <si>
+    <t>&lt;X=360&gt;&lt;Y=442&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Function=FormatNumber(text,2,,)&gt;</t>
+  </si>
+  <si>
+    <t>!&lt;CONCAT&gt;&lt;Employees Full Name&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Type=File&gt;&lt;File=PAY01.xlsx&gt;&lt;Sheet=SALERY DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=C&gt;</t>
+  </si>
+  <si>
+    <t>!&lt;CONCAT&gt;&lt;Employers' TIN&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Type=Text&gt;&lt;Text=&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Type=Text&gt;&lt;Text=TIN&gt;</t>
+  </si>
+  <si>
+    <t>Birth Day</t>
+  </si>
+  <si>
+    <t>&lt;Type=File&gt;&lt;File=EMP01.xlsx&gt;&lt;Sheet=PERSONAL DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=C&gt;</t>
+  </si>
+  <si>
+    <t>&lt;X=340&gt;&lt;Y=515&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Function=FormatDate(text,%Y/%m/%d)&gt;</t>
+  </si>
+  <si>
+    <t>Date of Join</t>
+  </si>
+  <si>
+    <t>&lt;Type=File&gt;&lt;File=EMP01.xlsx&gt;&lt;Sheet=PERSONAL DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=B&gt;</t>
+  </si>
+  <si>
+    <t>&lt;X=170&gt;&lt;Y=515&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Function=FormatDate(text,%d-%m-%Y)&gt;</t>
+  </si>
+  <si>
+    <t>Basic Salary in Words</t>
+  </si>
+  <si>
+    <t>&lt;Type=File&gt;&lt;File=PAY01.xlsx&gt;&lt;Sheet=SALERY DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=E&gt;</t>
+  </si>
+  <si>
+    <t>&lt;X=1.01in&gt;&lt;Y=8.2in&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;&lt;Function=SrinkToFit(4.2in,2)&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Function=NumberToText(text,Integer)&gt;</t>
+  </si>
+  <si>
+    <t>Basic Salary</t>
+  </si>
+  <si>
+    <t>&lt;X=25mm&gt;&lt;Y=215mm&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Function=NumberToCurrency(text,2,USD)&gt;</t>
+  </si>
+  <si>
+    <t>No Space Format Number Test</t>
+  </si>
+  <si>
+    <t>&lt;X=100mm&gt;&lt;Y=215mm&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Function=FormatNumber(text,2,USD,ONLY)&gt;</t>
+  </si>
+  <si>
     <t>SKIP</t>
   </si>
   <si>
-    <t>!&lt;CONCAT&gt;&lt;Employees Full Name&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Type=Text&gt;&lt;Text=&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Type=File&gt;&lt;File=PAY01.xlsx&gt;&lt;Sheet=SALERY DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=C&gt;</t>
-  </si>
-  <si>
-    <t>!&lt;CONCAT&gt;&lt;Employers' TIN&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Type=Text&gt;&lt;Text=TIN&gt;</t>
-  </si>
-  <si>
-    <t>Birth Day</t>
-  </si>
-  <si>
-    <t>&lt;Type=File&gt;&lt;File=EMP01.xlsx&gt;&lt;Sheet=PERSONAL DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=C&gt;</t>
-  </si>
-  <si>
-    <t>&lt;X=340&gt;&lt;Y=515&gt;</t>
-  </si>
-  <si>
-    <t>Date of Join</t>
-  </si>
-  <si>
-    <t>&lt;Type=File&gt;&lt;File=EMP01.xlsx&gt;&lt;Sheet=PERSONAL DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=B&gt;</t>
-  </si>
-  <si>
-    <t>&lt;X=170&gt;&lt;Y=515&gt;</t>
-  </si>
-  <si>
-    <t>Basic Salary in Words</t>
-  </si>
-  <si>
-    <t>&lt;Type=File&gt;&lt;File=PAY01.xlsx&gt;&lt;Sheet=SALERY DATA&gt;&lt;PrimeryKey=A&gt;&lt;Value=E&gt;</t>
-  </si>
-  <si>
-    <t>&lt;X=1.01in&gt;&lt;Y=8.2in&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;&lt;LineSpace=1.2X&gt;&lt;Function=SrinkToFit(4.2in,2)&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Function=NumberToText(text,Integer)&gt;</t>
-  </si>
-  <si>
-    <t>Basic Salary</t>
-  </si>
-  <si>
-    <t>&lt;X=25mm&gt;&lt;Y=215mm&gt;&lt;Font=Helvetica&gt;&lt;FontSize=12&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Function=NumberToCurrency(text,USD,2)&gt;</t>
-  </si>
-  <si>
     <t>Calibration 0 0</t>
   </si>
   <si>
@@ -227,6 +248,9 @@
     <t>Doe</t>
   </si>
   <si>
+    <t>John Doe</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
@@ -236,49 +260,65 @@
     <t>Smith</t>
   </si>
   <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
     <t>Michael</t>
   </si>
   <si>
     <t>Johnson</t>
   </si>
   <si>
+    <t>Michael Johnson</t>
+  </si>
+  <si>
     <t>Emily</t>
   </si>
   <si>
     <t>Brown</t>
   </si>
   <si>
+    <t>Emily Brown</t>
+  </si>
+  <si>
     <t>David</t>
   </si>
   <si>
     <t>Lee</t>
   </si>
   <si>
+    <t>David Lee</t>
+  </si>
+  <si>
     <t>Olivia</t>
   </si>
   <si>
     <t>Garcia</t>
   </si>
   <si>
-    <t>Zero</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>&lt;Type=Text&gt;&lt;Text=0.00&gt;</t>
-  </si>
-  <si>
-    <t>&lt;X=360&gt;&lt;Y=442&gt;</t>
+    <t>Olivia Garcia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -337,31 +377,50 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,85 +429,24 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -574,7 +572,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -583,7 +581,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -592,7 +590,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -666,7 +664,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -674,7 +672,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -692,7 +690,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -721,7 +719,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -746,7 +744,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -771,7 +769,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -796,7 +794,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -821,7 +819,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -846,7 +844,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -871,7 +869,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -896,7 +894,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -921,7 +919,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -934,15 +932,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -957,7 +949,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -965,7 +957,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -983,7 +975,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1008,7 +1000,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1033,7 +1025,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1058,7 +1050,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1083,7 +1075,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1108,7 +1100,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1133,7 +1125,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1158,7 +1150,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1183,7 +1175,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1208,7 +1200,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1221,15 +1213,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1243,7 +1229,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1261,7 +1247,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1290,7 +1276,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1315,7 +1301,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1340,7 +1326,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1365,7 +1351,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1390,7 +1376,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1415,7 +1401,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1440,7 +1426,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1465,7 +1451,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1490,7 +1476,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1503,413 +1489,424 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.45" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="62.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="90.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="45.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="6.17188" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.3516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="62.8516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="90.1719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.1719" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="13.5" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s" s="3">
         <v>7</v>
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" ht="13.5" customHeight="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s" s="3">
         <v>10</v>
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s" s="3">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s" s="3">
         <v>13</v>
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s" s="3">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s" s="3">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s" s="3">
         <v>16</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s" s="3">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s" s="3">
         <v>20</v>
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" ht="13.5" customHeight="1">
+      <c r="A7" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>24</v>
+      <c r="B8" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s" s="3">
+        <v>27</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" ht="13.5" customHeight="1">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>23</v>
+      <c r="B9" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s" s="3">
+        <v>29</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="3" t="s">
+      <c r="E9" t="s" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>26</v>
+      <c r="B10" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s" s="3">
+        <v>30</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" t="s" s="3">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" ht="15.45" customHeight="1">
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s" s="3">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s" s="3">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s" s="3">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" ht="15.45" customHeight="1">
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" t="s" s="3">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s" s="3">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s" s="3">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" ht="15.45" customHeight="1">
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="B14" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s" s="3">
         <v>40</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="D14" t="s" s="3">
         <v>44</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E14" t="s" s="3">
         <v>45</v>
       </c>
+    </row>
+    <row r="15" ht="15.45" customHeight="1">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s" s="3">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s" s="3">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s" s="3">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" ht="15.45" customHeight="1">
+      <c r="A16" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s" s="3">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s" s="3">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s" s="3">
+        <v>52</v>
+      </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>48</v>
+    <row r="17" ht="15.45" customHeight="1">
+      <c r="A17" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s" s="3">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s" s="3">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s" s="3">
+        <v>55</v>
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="3" t="s">
+    <row r="18" ht="15.45" customHeight="1">
+      <c r="A18" t="s" s="2">
         <v>49</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>51</v>
+      <c r="B18" t="s" s="3">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s" s="3">
+        <v>58</v>
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" ht="15.45" customHeight="1">
+      <c r="A19" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s" s="3">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="D19" t="s" s="3">
+        <v>61</v>
+      </c>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" ht="15.45" customHeight="1">
       <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s" s="3">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s" s="3">
+        <v>63</v>
+      </c>
+      <c r="D20" t="s" s="3">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" ht="15.45" customHeight="1">
       <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>57</v>
+      <c r="B21" t="s" s="3">
+        <v>65</v>
+      </c>
+      <c r="C21" t="s" s="3">
+        <v>27</v>
       </c>
       <c r="D21" s="3"/>
-      <c r="E21" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E21" t="s" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" ht="15.45" customHeight="1">
       <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>24</v>
+      <c r="B22" t="s" s="3">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s" s="3">
+        <v>67</v>
       </c>
       <c r="D22" s="3"/>
-      <c r="E22" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E22" t="s" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" ht="15.45" customHeight="1">
       <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>59</v>
+      <c r="B23" t="s" s="3">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s" s="3">
+        <v>27</v>
       </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E23" t="s" s="3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" ht="15.45" customHeight="1">
       <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B24" t="s" s="3">
+        <v>65</v>
+      </c>
+      <c r="C24" t="s" s="3">
+        <v>69</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" t="s" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" ht="15.45" customHeight="1">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3" t="s">
-        <v>60</v>
+      <c r="B25" t="s" s="3">
+        <v>65</v>
+      </c>
+      <c r="C25" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" t="s" s="3">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1917,171 +1914,170 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.45" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="4.85156" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.1719" style="6" customWidth="1"/>
+    <col min="3" max="3" width="13.3516" style="6" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" ht="13.5" customHeight="1">
+      <c r="A1" t="s" s="7">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="8">
+      <c r="B1" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s" s="7">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s" s="7">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s" s="7">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" ht="13.5" customHeight="1">
+      <c r="A2" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="B2" s="9">
         <v>14</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="6" t="str">
-        <f t="shared" ref="E2:E7" si="0">CONCATENATE(C2," ",D2)</f>
-        <v>John Doe</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="8">
+      <c r="C2" t="s" s="7">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s" s="7">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s" s="7">
+        <f>CONCATENATE(C2," ",D2)</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" ht="13.5" customHeight="1">
+      <c r="A3" t="s" s="8">
+        <v>79</v>
+      </c>
+      <c r="B3" s="9">
         <v>25</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Jane Smith</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="C3" t="s" s="7">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s" s="7">
+        <v>81</v>
+      </c>
+      <c r="E3" t="s" s="7">
+        <f>CONCATENATE(C3," ",D3)</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" ht="13.5" customHeight="1">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="9">
         <v>109</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Michael Johnson</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
+      <c r="C4" t="s" s="7">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s" s="7">
+        <v>84</v>
+      </c>
+      <c r="E4" t="s" s="7">
+        <f>CONCATENATE(C4," ",D4)</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" ht="13.5" customHeight="1">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="9">
         <v>120</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Emily Brown</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="C5" t="s" s="7">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s" s="7">
+        <v>87</v>
+      </c>
+      <c r="E5" t="s" s="7">
+        <f>CONCATENATE(C5," ",D5)</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" ht="13.5" customHeight="1">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="9">
         <v>123</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>David Lee</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+      <c r="C6" t="s" s="7">
+        <v>89</v>
+      </c>
+      <c r="D6" t="s" s="7">
+        <v>90</v>
+      </c>
+      <c r="E6" t="s" s="7">
+        <f>CONCATENATE(C6," ",D6)</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" ht="13.5" customHeight="1">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="9">
         <v>124</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Olivia Garcia</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="C7" t="s" s="7">
+        <v>92</v>
+      </c>
+      <c r="D7" t="s" s="7">
+        <v>93</v>
+      </c>
+      <c r="E7" t="s" s="7">
+        <f>CONCATENATE(C7," ",D7)</f>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" ht="13.5" customHeight="1">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" ht="13.5" customHeight="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" ht="13.5" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>